<commit_message>
Successfull optimization from class
</commit_message>
<xml_diff>
--- a/input/df_input_test.xlsx
+++ b/input/df_input_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02. Mestrado\TU Darmstadt\Energy Science and Engineering\5. Sommersemester 2023\Masterarbeit\5. Thesis\3. Python Routine\masterthesis\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07606721-44C5-481D-ABEC-A5F267D48DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046506B8-61BD-4436-811E-2151DC37833F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>HOURS</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>cost_y</t>
+  </si>
+  <si>
+    <t>demand</t>
   </si>
 </sst>
 </file>
@@ -363,15 +366,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,8 +384,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2">
         <v>1</v>
       </c>
@@ -392,8 +398,11 @@
       <c r="C2">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -404,8 +413,11 @@
       <c r="C3">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f t="shared" ref="A4:A25" si="0">A3+1</f>
         <v>3</v>
@@ -416,8 +428,11 @@
       <c r="C4">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -428,8 +443,11 @@
       <c r="C5">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -440,8 +458,12 @@
       <c r="C6">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D6">
+        <v>59</v>
+      </c>
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -452,8 +474,11 @@
       <c r="C7">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D7">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -464,8 +489,11 @@
       <c r="C8">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -476,8 +504,11 @@
       <c r="C9">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -488,8 +519,11 @@
       <c r="C10">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D10">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -500,8 +534,11 @@
       <c r="C11">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D11">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -512,8 +549,11 @@
       <c r="C12">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D12">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -524,8 +564,11 @@
       <c r="C13">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D13">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -536,8 +579,11 @@
       <c r="C14">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D14">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -548,8 +594,11 @@
       <c r="C15">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -560,8 +609,11 @@
       <c r="C16">
         <v>0.45</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -572,8 +624,11 @@
       <c r="C17">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -584,8 +639,11 @@
       <c r="C18">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -596,8 +654,11 @@
       <c r="C19">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -608,8 +669,11 @@
       <c r="C20">
         <v>0.47</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -620,8 +684,11 @@
       <c r="C21">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D21">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -632,8 +699,11 @@
       <c r="C22">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D22">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -644,8 +714,11 @@
       <c r="C23">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D23">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -656,8 +729,11 @@
       <c r="C24">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="D24">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -667,6 +743,9 @@
       </c>
       <c r="C25">
         <v>0.41</v>
+      </c>
+      <c r="D25">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>